<commit_message>
commented business requirements / rules on Transaction statistics
</commit_message>
<xml_diff>
--- a/.ph/2022-04-07 Peppol Reporting Requirements Draft.xlsx
+++ b/.ph/2022-04-07 Peppol Reporting Requirements Draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\svn-philip\OpenPeppol\Reporting\BIS\2022-01-14 Input Philip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerou\develop\OpenPEPPOL\Specs\reporting\.ph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD86C5E0-6E24-4B0E-A305-15288E744493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DC15E-6B85-4111-B13C-5CCE3F992A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D55973C5-EE73-483F-94E6-D9DE17C4B093}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{D55973C5-EE73-483F-94E6-D9DE17C4B093}"/>
   </bookViews>
   <sheets>
     <sheet name="End User Reporting" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="168">
   <si>
     <t>ID</t>
   </si>
@@ -471,13 +471,133 @@
   </si>
   <si>
     <t>The exchange date in UTC timezone must be &gt;= the reporting period start date (BR-TS-02) and &lt;= the reporting period end date (BR-TS-03)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Req of SP / Part of BIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture Assumption </t>
+  </si>
+  <si>
+    <t>simplified to YYYY-MM</t>
+  </si>
+  <si>
+    <t>Questions / Pending Decisions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Architecture Assumption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Edge case for new Service Providers</t>
+    </r>
+  </si>
+  <si>
+    <t>This is not part of the IR, can be omitted</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Req</t>
+  </si>
+  <si>
+    <t>Req / Part of Process Section</t>
+  </si>
+  <si>
+    <t>Req/ Scope</t>
+  </si>
+  <si>
+    <t>Architectural Clarification</t>
+  </si>
+  <si>
+    <t>Req / Scope</t>
+  </si>
+  <si>
+    <t>Req / Process</t>
+  </si>
+  <si>
+    <t>Architectural Clarification, does it need to be in the BIS?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Architectural Clarification, BIS concerns only </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Successful Business Transactions.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Does it need to be in the BIS?</t>
+    </r>
+  </si>
+  <si>
+    <t>Req / Message Content</t>
+  </si>
+  <si>
+    <t>Part of the BIS Document, part of the Process</t>
+  </si>
+  <si>
+    <t>Dataset comes the IR, can we change it to Successful Transaction?</t>
+  </si>
+  <si>
+    <t>Initial High-Level Requirement from IR 4.4</t>
+  </si>
+  <si>
+    <t>Architecture Clarification / How should the AP instances with Same Certs be handled?</t>
+  </si>
+  <si>
+    <t>Redundant Requirement aleady exists in Data Gathering (row 9)</t>
+  </si>
+  <si>
+    <t>Redundant Requirement already exists in Data Gathering (row 9)</t>
+  </si>
+  <si>
+    <t>Rule / Message / Schema</t>
+  </si>
+  <si>
+    <t>Fixed value of the receiver. Part of Message? Only SBDH?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +615,23 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -557,9 +694,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,7 +716,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -877,7 +1018,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" style="1" customWidth="1"/>
@@ -1356,22 +1497,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E621EE-7927-4611-8825-097D75EE6168}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1388,8 +1531,14 @@
         <v>7</v>
       </c>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1399,14 +1548,20 @@
       <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1419,8 +1574,17 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1433,8 +1597,17 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -1448,13 +1621,19 @@
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>148</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -1470,8 +1649,14 @@
       <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1484,8 +1669,12 @@
       <c r="F7" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1501,8 +1690,12 @@
       <c r="F8" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -1515,8 +1708,14 @@
       <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -1530,8 +1729,14 @@
       <c r="F10" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1545,8 +1750,14 @@
       <c r="F11" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -1560,8 +1771,14 @@
       <c r="F12" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1577,8 +1794,11 @@
       <c r="F13" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G13" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1594,8 +1814,14 @@
       <c r="F14" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G14" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -1611,8 +1837,14 @@
       <c r="F15" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1628,8 +1860,14 @@
       <c r="F16" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G16" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1645,8 +1883,14 @@
       <c r="F17" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G17" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -1662,8 +1906,14 @@
       <c r="F18" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -1679,8 +1929,14 @@
       <c r="F19" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G19" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1696,8 +1952,14 @@
       <c r="F20" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G20" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1713,8 +1975,14 @@
       <c r="F21" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1724,19 +1992,34 @@
       <c r="D22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -1744,7 +2027,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1755,7 +2038,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -1766,7 +2049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +2057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -1782,7 +2065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>11</v>
       </c>
@@ -1790,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1804,7 +2087,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -1817,8 +2100,14 @@
       <c r="F31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="G31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -1834,8 +2123,11 @@
       <c r="F32" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G32" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -1851,8 +2143,11 @@
       <c r="F33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G33" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>3</v>
       </c>
@@ -1868,8 +2163,11 @@
       <c r="F34" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G34" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -1879,8 +2177,14 @@
       <c r="F35" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G35" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -1893,30 +2197,45 @@
       <c r="F36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G36" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
       <c r="F37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>87</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added EUR Schematron; #39
</commit_message>
<xml_diff>
--- a/.ph/2022-04-07 Peppol Reporting Requirements Draft.xlsx
+++ b/.ph/2022-04-07 Peppol Reporting Requirements Draft.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerou\develop\OpenPEPPOL\Specs\reporting\.ph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\reporting\.ph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DC15E-6B85-4111-B13C-5CCE3F992A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395ED4C7-E74C-43A5-8A0D-2643B55485C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{D55973C5-EE73-483F-94E6-D9DE17C4B093}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D55973C5-EE73-483F-94E6-D9DE17C4B093}"/>
   </bookViews>
   <sheets>
     <sheet name="End User Reporting" sheetId="1" r:id="rId1"/>
-    <sheet name="Transaction Statistics" sheetId="3" r:id="rId2"/>
+    <sheet name="EUR Rules" sheetId="5" r:id="rId2"/>
+    <sheet name="Transaction Statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="TS Rules" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="205">
   <si>
     <t>ID</t>
   </si>
@@ -432,16 +434,7 @@
     <t>BR-EUR-30</t>
   </si>
   <si>
-    <t>The Reporting Period Start Date must be provided in the Report</t>
-  </si>
-  <si>
-    <t>The Reporting Period End Date must be provided in the Report</t>
-  </si>
-  <si>
     <t>If a Service Provider ends its Peppol activities the report must be send as the last action.</t>
-  </si>
-  <si>
-    <t>If a Service Provider ends its Peppol activities during a reporting period, this particular reporting period ends for this Service Provider at the ending point in time.</t>
   </si>
   <si>
     <t>Only data from the Peppol production network must be reported</t>
@@ -488,36 +481,7 @@
     <t>Questions / Pending Decisions</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Architecture Assumption</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / Edge case for new Service Providers</t>
-    </r>
-  </si>
-  <si>
-    <t>This is not part of the IR, can be omitted</t>
-  </si>
-  <si>
     <t>Rule</t>
-  </si>
-  <si>
-    <t>Req</t>
   </si>
   <si>
     <t>Req / Part of Process Section</t>
@@ -584,13 +548,142 @@
     <t>Redundant Requirement aleady exists in Data Gathering (row 9)</t>
   </si>
   <si>
-    <t>Redundant Requirement already exists in Data Gathering (row 9)</t>
-  </si>
-  <si>
     <t>Rule / Message / Schema</t>
   </si>
   <si>
     <t>Fixed value of the receiver. Part of Message? Only SBDH?</t>
+  </si>
+  <si>
+    <t>The Reporting Period must be provided in the Report</t>
+  </si>
+  <si>
+    <t>The Report needs to contain an identification of the specification it conforms to.</t>
+  </si>
+  <si>
+    <t>The Report must contain an identification of the specification it conforms to.</t>
+  </si>
+  <si>
+    <t>The Report must contain an identification of the business process context it appears in.</t>
+  </si>
+  <si>
+    <t>The Report must uniquely identify the reporting Service Provider.</t>
+  </si>
+  <si>
+    <t>Each country code reported, must be specified following the ISO-3166-1 Alpha2 code list.</t>
+  </si>
+  <si>
+    <t>The Report must contain the year and the month in which the reported data was gathered.</t>
+  </si>
+  <si>
+    <t>The Report must use UTC as the underlying timezone.</t>
+  </si>
+  <si>
+    <t>The Report must contain the legal identifier of every reported Intermediary of any End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain the legal name of every reported Intermediary of any End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain the country code of every reported Intermediary of any End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain the details of no, one or multiple End Users.</t>
+  </si>
+  <si>
+    <t>The Report must contain the legal identifier of every reported End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain the legal name of every reported End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain the country code of every reported End User.</t>
+  </si>
+  <si>
+    <t>The Report must contain an enumeration of all Dataset Type IDs sent out on behalf the End User in the reporting period.</t>
+  </si>
+  <si>
+    <t>Each Dataset Type IDs sent out on behalf the End User in the reporting period, must be present no more than once in the Report.</t>
+  </si>
+  <si>
+    <t>Each Dataset Type IDs sent out on behalf the End User in the reporting period, must be reported with identifier scheme and identifier value.</t>
+  </si>
+  <si>
+    <t>The Report must contain an enumeration of all Dataset Type IDs received on behalf the End User in the reporting period.</t>
+  </si>
+  <si>
+    <t>Each Dataset Type IDs received on behalf the End User in the reporting period, must be present no more than once in the Report.</t>
+  </si>
+  <si>
+    <t>Each Dataset Type IDs received on behalf the End User in the reporting period, must be reported with identifier scheme and identifier value.</t>
+  </si>
+  <si>
+    <t>The Report must contain an enumeration of all Peppol Participant IDs used by an End User in the reporting period.</t>
+  </si>
+  <si>
+    <t>Each Peppol Participant IDs used by an End User in the reporting period, must be reported with identifier scheme and identifier value.</t>
+  </si>
+  <si>
+    <t>BR-TS-06</t>
+  </si>
+  <si>
+    <t>BR-TS-07</t>
+  </si>
+  <si>
+    <t>BR-TS-08</t>
+  </si>
+  <si>
+    <t>BR-TS-09</t>
+  </si>
+  <si>
+    <t>BR-TS-10</t>
+  </si>
+  <si>
+    <t>BR-TS-11</t>
+  </si>
+  <si>
+    <t>BR-TS-12</t>
+  </si>
+  <si>
+    <t>BR-TS-13</t>
+  </si>
+  <si>
+    <t>BR-TS-14</t>
+  </si>
+  <si>
+    <t>BR-TS-15</t>
+  </si>
+  <si>
+    <t>BR-TS-16</t>
+  </si>
+  <si>
+    <t>BR-TS-17</t>
+  </si>
+  <si>
+    <t>BR-TS-18</t>
+  </si>
+  <si>
+    <t>BR-TS-19</t>
+  </si>
+  <si>
+    <t>BR-TS-20</t>
+  </si>
+  <si>
+    <t>BR-TS-21</t>
+  </si>
+  <si>
+    <t>BR-TS-22</t>
+  </si>
+  <si>
+    <t>The Report must not not contain timezone information for the reporting period.</t>
+  </si>
+  <si>
+    <t>The scheme for identifying the reporting Service Provider must follow the "Reporter ID Scheme" code list</t>
+  </si>
+  <si>
+    <t>If the Reporter ID scheme is set to "CertSubjectCN", the Reporter ID must be a valiid Peppol seat ID.</t>
+  </si>
+  <si>
+    <t>XSD only</t>
   </si>
 </sst>
 </file>
@@ -700,7 +793,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,7 +809,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1014,11 +1107,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C741F7-6BBF-4ADB-8698-A3300C1159E8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" style="1" customWidth="1"/>
@@ -1496,14 +1589,243 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E621EE-7927-4611-8825-097D75EE6168}">
-  <dimension ref="A1:H38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3969E37-D11D-43C2-8EAA-B7E2EA338EF9}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="85.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E621EE-7927-4611-8825-097D75EE6168}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.140625" style="1" customWidth="1"/>
@@ -1532,16 +1854,13 @@
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>95</v>
-      </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -1558,102 +1877,89 @@
         <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>146</v>
       </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>98</v>
-      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>148</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>149</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>99</v>
-      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1661,187 +1967,197 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="G7" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="7"/>
+        <v>150</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>134</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>142</v>
+      <c r="C13" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>136</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1849,393 +2165,460 @@
         <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>66</v>
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F30" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G30" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>88</v>
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="120" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F33" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="34" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F34" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB955338-4C1E-487A-8F9C-B3643191810A}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="85.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>167</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>